<commit_message>
plot week by week
</commit_message>
<xml_diff>
--- a/ParameterNameList/parameterList_task_OIS.xlsx
+++ b/ParameterNameList/parameterList_task_OIS.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Masud_OxfordCognition\Project13_ECT\OxCog_analysis_ECT\ParameterNameList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Masud_OxfordCognition\Project02_prolific\OxCog_analysis_ProlificControl\ParameterNameList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCBC214-11A9-42A5-959D-D72D83EACA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00959D8E-D9EA-4473-9AF2-D4F0615EC6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="4104" windowWidth="17172" windowHeight="12120" xr2:uid="{89D9FAA3-7342-4980-AE9A-5347263E0025}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{89D9FAA3-7342-4980-AE9A-5347263E0025}"/>
   </bookViews>
   <sheets>
-    <sheet name="all (2)" sheetId="6" r:id="rId1"/>
-    <sheet name="all" sheetId="3" r:id="rId2"/>
+    <sheet name="all" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Immediate object accuracy (%)</t>
   </si>
@@ -43,88 +42,58 @@
     <t>Delayed object accuracy (%)</t>
   </si>
   <si>
-    <t>Change in object accuracy (%)</t>
-  </si>
-  <si>
     <t>plist</t>
   </si>
   <si>
     <t>nlist</t>
   </si>
   <si>
-    <t>Proportion Error due to familiar object (%)</t>
-  </si>
-  <si>
-    <t>Proportion Error due to novel object (%)</t>
-  </si>
-  <si>
-    <t>Target Detection (%)</t>
-  </si>
-  <si>
-    <t>OIS_ImmediateObjectAccuracy</t>
-  </si>
-  <si>
-    <t>OIS_DelayedObjectAccuracy</t>
-  </si>
-  <si>
-    <t>OIS_Mismatching_FamiliarObject</t>
-  </si>
-  <si>
-    <t>OIS_Guessing_NovelObject</t>
-  </si>
-  <si>
-    <t>OIS_ImmediateLocationError</t>
-  </si>
-  <si>
-    <t>OIS_DelayedLocationError</t>
-  </si>
-  <si>
-    <t>OIS_change_in_ObjectAccuracy</t>
-  </si>
-  <si>
-    <t>OIS_change_in_LocationError</t>
-  </si>
-  <si>
-    <t>Change in location error (cm)</t>
-  </si>
-  <si>
     <t>Delayed location error (cm)</t>
   </si>
   <si>
     <t>Immediate location error (cm)</t>
   </si>
   <si>
-    <t>OIS_change_in_SemanticAccuracy</t>
-  </si>
-  <si>
-    <t>Change in semantic accuracy (%)</t>
-  </si>
-  <si>
     <t>Delayed semantic accuracy (%)</t>
   </si>
   <si>
     <t>Immediate semantic accuracy (%)</t>
   </si>
   <si>
-    <t>OIS_ImmediateSemanticAccuracy</t>
-  </si>
-  <si>
-    <t>OIS_DelayedSemanticAccuracy</t>
-  </si>
-  <si>
-    <t>OIS_TargetDetection</t>
-  </si>
-  <si>
     <t>typelist</t>
   </si>
   <si>
     <t>num</t>
   </si>
   <si>
-    <t>testTime_ois</t>
-  </si>
-  <si>
-    <t>time</t>
+    <t>ois_ImmediateObjectAccuracy</t>
+  </si>
+  <si>
+    <t>ois_ImmediateSemanticAccuracy</t>
+  </si>
+  <si>
+    <t>ois_ImmediateLocationError</t>
+  </si>
+  <si>
+    <t>ois_DelayedObjectAccuracy</t>
+  </si>
+  <si>
+    <t>ois_DelayedSemanticAccuracy</t>
+  </si>
+  <si>
+    <t>ois_DelayedLocationError</t>
+  </si>
+  <si>
+    <t>ois_rt_identification_immediate</t>
+  </si>
+  <si>
+    <t>ois_rt_localisation_immediate</t>
+  </si>
+  <si>
+    <t>ois_rt_identification_delayed</t>
+  </si>
+  <si>
+    <t>ois_rt_localisation_delayed</t>
   </si>
 </sst>
 </file>
@@ -475,94 +444,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4309F23D-3A81-4038-870E-52FA89B5AC1C}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EC45A0-751D-429E-9211-6A1DA8931C9E}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EC45A0-751D-429E-9211-6A1DA8931C9E}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,68 +460,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -643,76 +529,42 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>